<commit_message>
Update Test Case Clocking In and Out for User
</commit_message>
<xml_diff>
--- a/Data Files/Data User.xlsx
+++ b/Data Files/Data User.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mufti\Data\SQA RPA\Coding\Hadir App Katalon Testing\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED3AE27-17AE-4DAC-9641-3CBFF598B067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8316945-F78A-4036-9AC1-11F5651F711C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="invalid_login" sheetId="1" r:id="rId1"/>
     <sheet name="invalid_email_format" sheetId="2" r:id="rId2"/>
     <sheet name="clocking_in_selfie" sheetId="3" r:id="rId3"/>
-    <sheet name="clocking_in_nonselfie" sheetId="4" r:id="rId4"/>
+    <sheet name="clocking_in_non_selfie" sheetId="6" r:id="rId4"/>
     <sheet name="clocking_out" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>email</t>
   </si>
@@ -85,25 +85,22 @@
     <t>note</t>
   </si>
   <si>
-    <t>testuser4@gmail.com</t>
-  </si>
-  <si>
-    <t>testuser5@gmail.com</t>
-  </si>
-  <si>
     <t>absen masuk selfie pakai note</t>
   </si>
   <si>
-    <t>noselfieuser5@gmail.com</t>
-  </si>
-  <si>
-    <t>noselfieuser6@gmail.com</t>
-  </si>
-  <si>
     <t>absen masuk non-selfie pakai note</t>
   </si>
   <si>
     <t>berhasil melakukan absen keluar</t>
+  </si>
+  <si>
+    <t>testuser2@gmail.com</t>
+  </si>
+  <si>
+    <t>noselfieuser@gmail.com</t>
+  </si>
+  <si>
+    <t>noselfieuser2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -526,7 +523,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +593,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,19 +615,19 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
+      <c r="A2" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>12345678</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
         <v>12345678</v>
@@ -639,24 +636,25 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{7A6C80E8-EFC2-4F83-99AB-19CD1612806B}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{9EEC10BD-D9D1-4E58-A822-7B3E4515E0E5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C63F06-C99A-4508-B11F-DED5CC88E820}">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A2F633-6B69-44AF-B9FE-4861BF92B752}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -671,43 +669,29 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>21</v>
+      <c r="A2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{F03DB3A8-17F4-4E04-9E50-76030EA7100A}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{5EAC2133-86AD-4003-88B5-9DBFFE5FA58D}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{4D3093A7-E9FC-4308-9403-A3A4D3660CD2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -717,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD99258-554D-46AC-B79A-8B6EEC354E53}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,25 +724,29 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
+      <c r="A2" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B2">
         <v>12345678</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
+      <c r="A3" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B3">
         <v>12345678</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{4E08E968-C670-468F-9300-D3CDC34CDAB8}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{955E1D73-07F3-4677-AE8D-86ADE470F331}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>